<commit_message>
finalization - write header info to correct cells, output_template updated
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>F L I G H T   L I S T</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>SSR</t>
+  </si>
+  <si>
+    <t>flight-date</t>
+  </si>
+  <si>
+    <t>flight number</t>
+  </si>
+  <si>
+    <t>routing</t>
+  </si>
+  <si>
+    <t>adults+infants</t>
   </si>
 </sst>
 </file>
@@ -69,24 +81,18 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -166,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +185,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5B8B7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -362,10 +362,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0"/>
@@ -377,8 +378,8 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0"/>
@@ -390,7 +391,6 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
@@ -413,9 +413,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,6 +420,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="20 % – Zvýraznění1 2" xfId="13"/>
@@ -520,7 +520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -555,7 +555,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -764,27 +764,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G194"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A5:E194"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="17" style="13" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17" style="12" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7"/>
@@ -794,12 +794,19 @@
     </row>
     <row r="2" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1529,83 +1536,82 @@
       <c r="C144"/>
       <c r="D144"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="C145"/>
       <c r="D145"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146"/>
       <c r="C146"/>
       <c r="D146"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147"/>
       <c r="C147"/>
       <c r="D147"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148"/>
       <c r="C148"/>
       <c r="D148"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149"/>
       <c r="C149"/>
       <c r="D149"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150"/>
       <c r="C150"/>
       <c r="D150"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151"/>
       <c r="C151"/>
       <c r="D151"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152"/>
       <c r="C152"/>
       <c r="D152"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153"/>
       <c r="C153"/>
       <c r="D153"/>
-      <c r="E153"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154"/>
       <c r="C154"/>
       <c r="D154"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155"/>
       <c r="C155"/>
       <c r="D155"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156"/>
       <c r="C156"/>
       <c r="D156"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157"/>
       <c r="C157"/>
       <c r="D157"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158"/>
       <c r="C158"/>
       <c r="D158"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159"/>
       <c r="C159"/>
       <c r="D159"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160"/>
       <c r="C160"/>
       <c r="D160"/>
@@ -1775,14 +1781,10 @@
       <c r="C193"/>
       <c r="D193"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194"/>
-      <c r="C194"/>
-      <c r="D194"/>
-    </row>
   </sheetData>
   <autoFilter ref="A4:F196"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>